<commit_message>
Add USC convocatorias URL to scraper configuration
Co-authored-by: PabloskyPP <182076036+PabloskyPP@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/scraper_estudios.xlsx
+++ b/data/scraper_estudios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,66 @@
           <t>url</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>contenido_colaborar</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>contenido_contratación</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>contenido_investigación</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>contenido_persoal</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>contenido_proxecto</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>contenido_proxectos</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>titulo_colaborar</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>titulo_contratación</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>titulo_investigación</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>titulo_persoal</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>titulo_proxecto</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>titulo_proxectos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -485,6 +545,128 @@
         <is>
           <t>https://www.usc.gal/gl/emprego</t>
         </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>UVigoProfesor</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-10-09 16:29:09</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://secretaria.uvigo.gal/uv/web/convocatoria/public/index</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>USCEmprego</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-10-09 16:29:09</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.usc.gal/gl/emprego</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USCConvocatorias</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-10-09 16:29:09</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://www.usc.gal/gl/investigar-na-usc/convocatorias</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>12</v>
+      </c>
+      <c r="H6" t="n">
+        <v>12</v>
+      </c>
+      <c r="I6" t="n">
+        <v>12</v>
+      </c>
+      <c r="J6" t="n">
+        <v>12</v>
+      </c>
+      <c r="K6" t="n">
+        <v>12</v>
+      </c>
+      <c r="L6" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" t="n">
+        <v>12</v>
+      </c>
+      <c r="N6" t="n">
+        <v>12</v>
+      </c>
+      <c r="O6" t="n">
+        <v>12</v>
+      </c>
+      <c r="P6" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final verification: USC convocatorias scraping working correctly
Co-authored-by: PabloskyPP <182076036+PabloskyPP@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/scraper_estudios.xlsx
+++ b/data/scraper_estudios.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,18 +568,6 @@
           <t>https://secretaria.uvigo.gal/uv/web/convocatoria/public/index</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -602,18 +590,6 @@
           <t>https://www.usc.gal/gl/emprego</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -621,7 +597,6 @@
           <t>USCConvocatorias</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>2025-10-09 16:29:09</t>
@@ -666,6 +641,128 @@
         <v>12</v>
       </c>
       <c r="P6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>UVigoProfesor</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-10-09 16:30:19</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://secretaria.uvigo.gal/uv/web/convocatoria/public/index</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>USCEmprego</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-10-09 16:30:19</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://www.usc.gal/gl/emprego</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>USCConvocatorias</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-10-09 16:30:19</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.usc.gal/gl/investigar-na-usc/convocatorias</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12</v>
+      </c>
+      <c r="J9" t="n">
+        <v>12</v>
+      </c>
+      <c r="K9" t="n">
+        <v>12</v>
+      </c>
+      <c r="L9" t="n">
+        <v>10</v>
+      </c>
+      <c r="M9" t="n">
+        <v>12</v>
+      </c>
+      <c r="N9" t="n">
+        <v>12</v>
+      </c>
+      <c r="O9" t="n">
+        <v>12</v>
+      </c>
+      <c r="P9" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>